<commit_message>
removing employee_id columns and gracefully closing db connection
</commit_message>
<xml_diff>
--- a/deliverables/test/test.xlsx
+++ b/deliverables/test/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="12435" windowHeight="9540" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="12435" windowHeight="9540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="employees" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>Bob</t>
   </si>
@@ -42,9 +42,6 @@
     <t>State</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>First</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>Age</t>
   </si>
   <si>
-    <t>Employee Id</t>
-  </si>
-  <si>
     <t>Zip code</t>
   </si>
   <si>
@@ -78,9 +72,6 @@
     <t>Ny</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>Score 1</t>
   </si>
   <si>
@@ -88,6 +79,9 @@
   </si>
   <si>
     <t>Score 3</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -422,23 +416,23 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -492,19 +486,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -513,7 +507,7 @@
         <v>7</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -521,10 +515,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>6492</v>
@@ -535,10 +529,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>94203</v>
@@ -549,10 +543,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>11215</v>
@@ -566,83 +560,70 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>78.612399999999994</v>
       </c>
       <c r="C2">
-        <v>78.612399999999994</v>
+        <v>93.119100000000003</v>
       </c>
       <c r="D2">
-        <v>93.119100000000003</v>
-      </c>
-      <c r="E2">
         <v>92.004499999999993</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>84.92</v>
       </c>
       <c r="C3">
-        <v>84.92</v>
+        <v>90</v>
       </c>
       <c r="D3">
-        <v>90</v>
-      </c>
-      <c r="E3">
         <v>99.2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>100</v>
       </c>
       <c r="C4">
-        <v>100</v>
+        <v>67.634500000000003</v>
       </c>
       <c r="D4">
-        <v>67.634500000000003</v>
-      </c>
-      <c r="E4">
         <v>2.3333300000000001</v>
       </c>
     </row>

</xml_diff>